<commit_message>
Modification du ReadMe, Gantt, Makefile
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -89,9 +89,6 @@
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">Version SDL2</t>
-  </si>
-  <si>
     <t xml:space="preserve">2.1</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t xml:space="preserve">2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version SDL2</t>
   </si>
   <si>
     <t xml:space="preserve">Test/ Doc</t>
@@ -753,13 +753,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:IV25"/>
+  <dimension ref="A1:IV30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
@@ -3950,21 +3950,6 @@
       <c r="A16" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="37" t="n">
-        <v>44966</v>
-      </c>
-      <c r="E16" s="38" t="n">
-        <v>44994</v>
-      </c>
-      <c r="F16" s="39" t="n">
-        <f aca="false">MAX(E17:E20)-D16</f>
-        <v>28</v>
-      </c>
-      <c r="G16" s="40"/>
       <c r="H16" s="41"/>
       <c r="I16" s="42"/>
       <c r="J16" s="41"/>
@@ -4217,20 +4202,8 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="37" t="n">
-        <v>44966</v>
-      </c>
-      <c r="E17" s="38" t="n">
-        <v>44994</v>
-      </c>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+        <v>21</v>
+      </c>
       <c r="H17" s="49"/>
       <c r="I17" s="50"/>
       <c r="J17" s="49"/>
@@ -4483,20 +4456,8 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="37" t="n">
-        <v>44966</v>
-      </c>
-      <c r="E18" s="38" t="n">
-        <v>44994</v>
-      </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+        <v>22</v>
+      </c>
       <c r="H18" s="49"/>
       <c r="I18" s="50"/>
       <c r="J18" s="49"/>
@@ -4749,20 +4710,8 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="37" t="n">
-        <v>44966</v>
-      </c>
-      <c r="E19" s="38" t="n">
-        <v>44994</v>
-      </c>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
+        <v>23</v>
+      </c>
       <c r="H19" s="49"/>
       <c r="I19" s="50"/>
       <c r="J19" s="49"/>
@@ -5015,20 +4964,8 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="37" t="n">
-        <v>44966</v>
-      </c>
-      <c r="E20" s="38" t="n">
-        <v>44994</v>
-      </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
+        <v>24</v>
+      </c>
       <c r="H20" s="49"/>
       <c r="I20" s="50"/>
       <c r="J20" s="49"/>
@@ -5280,20 +5217,19 @@
       <c r="IV20" s="33"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34" t="s">
-        <v>27</v>
-      </c>
       <c r="B21" s="35" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21" s="36"/>
-      <c r="D21" s="38" t="n">
+      <c r="D21" s="37" t="n">
+        <v>44966</v>
+      </c>
+      <c r="E21" s="38" t="n">
         <v>44994</v>
       </c>
-      <c r="E21" s="38"/>
       <c r="F21" s="39" t="n">
         <f aca="false">MAX(E22:E25)-D21</f>
-        <v>-44994</v>
+        <v>28</v>
       </c>
       <c r="G21" s="40"/>
       <c r="H21" s="41"/>
@@ -5547,13 +5483,16 @@
       <c r="IV21" s="33"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="45"/>
+      <c r="B22" s="45" t="s">
+        <v>13</v>
+      </c>
       <c r="C22" s="46"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="53"/>
+      <c r="D22" s="37" t="n">
+        <v>44966</v>
+      </c>
+      <c r="E22" s="38" t="n">
+        <v>44994</v>
+      </c>
       <c r="F22" s="47"/>
       <c r="G22" s="48"/>
       <c r="H22" s="49"/>
@@ -5807,13 +5746,16 @@
       <c r="IV22" s="33"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="45"/>
+      <c r="B23" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="C23" s="46"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
+      <c r="D23" s="37" t="n">
+        <v>44966</v>
+      </c>
+      <c r="E23" s="38" t="n">
+        <v>44994</v>
+      </c>
       <c r="F23" s="47"/>
       <c r="G23" s="48"/>
       <c r="H23" s="49"/>
@@ -6067,13 +6009,16 @@
       <c r="IV23" s="33"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="45"/>
+      <c r="B24" s="45" t="s">
+        <v>17</v>
+      </c>
       <c r="C24" s="46"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="53"/>
+      <c r="D24" s="37" t="n">
+        <v>44966</v>
+      </c>
+      <c r="E24" s="38" t="n">
+        <v>44994</v>
+      </c>
       <c r="F24" s="47"/>
       <c r="G24" s="48"/>
       <c r="H24" s="49"/>
@@ -6327,13 +6272,16 @@
       <c r="IV24" s="33"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="45"/>
+      <c r="B25" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="C25" s="46"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
+      <c r="D25" s="37" t="n">
+        <v>44966</v>
+      </c>
+      <c r="E25" s="38" t="n">
+        <v>44994</v>
+      </c>
       <c r="F25" s="47"/>
       <c r="G25" s="48"/>
       <c r="H25" s="49"/>
@@ -6586,6 +6534,68 @@
       <c r="IU25" s="33"/>
       <c r="IV25" s="33"/>
     </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="36"/>
+      <c r="D26" s="38" t="n">
+        <v>44994</v>
+      </c>
+      <c r="E26" s="38"/>
+      <c r="F26" s="39" t="n">
+        <f aca="false">MAX(E27:E30)-D26</f>
+        <v>-44994</v>
+      </c>
+      <c r="G26" s="40"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="45"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="45"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="48"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="45"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="48"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="45"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="48"/>
+    </row>
   </sheetData>
   <mergeCells count="34">
     <mergeCell ref="L9:R9"/>

</xml_diff>